<commit_message>
0128    console.table跑通，，，，cli table3添加 validation修改，，，，oxide.ts添加
</commit_message>
<xml_diff>
--- a/packages/模块进度.xlsx
+++ b/packages/模块进度.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\project\js\AnJsflScript-ts\packages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C7E896-7787-4644-ACA2-355CCB7622F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF7EEE9-AAFA-4B96-84E1-73A3F3632683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="25720" windowHeight="13800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9839,8 +9839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29BB500-F51A-4269-B6E7-D25BB2E2A352}">
   <dimension ref="C4:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -9933,8 +9933,8 @@
       <c r="C16" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="3:6" ht="19.5">
       <c r="C17" s="1"/>
@@ -10036,6 +10036,7 @@
         <v>182</v>
       </c>
       <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>